<commit_message>
update to data import from 1) proform to get more data and move any clearning to R/03 and 2) to create a single large file with betfair win/place data
</commit_message>
<xml_diff>
--- a/data/proform_sql_layout.xlsx
+++ b/data/proform_sql_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Projects\horse-racing-place-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D64B604-C31C-498D-B883-C7F1181779E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55337F3C-34FF-4097-8429-76F37B4922F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{0338094F-6C0F-429B-B4B9-4546631CB8E6}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{0338094F-6C0F-429B-B4B9-4546631CB8E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB88D54-9412-489A-99BB-F362968D19E0}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>